<commit_message>
modified the import for documents and updated the XLS with correct information
</commit_message>
<xml_diff>
--- a/CMDSReports.xlsx
+++ b/CMDSReports.xlsx
@@ -34,9 +34,6 @@
     <t>Average Case Completion - ALJ.jasper</t>
   </si>
   <si>
-    <t>Year, ALJ</t>
-  </si>
-  <si>
     <t>Average Case Completion - All</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>Cases Stayed - ALJ.jasper</t>
   </si>
   <si>
-    <t>ALJ</t>
-  </si>
-  <si>
     <t>Cases Stayed - All</t>
   </si>
   <si>
@@ -226,9 +220,6 @@
     <t>RR Completion in Days - By ALJ</t>
   </si>
   <si>
-    <t>RR Completion Days by ALJ.jasper</t>
-  </si>
-  <si>
     <t>RR Completion in Days - ALL</t>
   </si>
   <si>
@@ -250,7 +241,16 @@
     <t>Scheduled Hearings.jasper</t>
   </si>
   <si>
-    <t>begin date, end date, ALJ</t>
+    <t>Year, InvestigatorID</t>
+  </si>
+  <si>
+    <t>InvestigatorID</t>
+  </si>
+  <si>
+    <t>begin date, end date, InvestigatorID</t>
+  </si>
+  <si>
+    <t>RR Completion Days - ALJ.jasper</t>
   </si>
 </sst>
 </file>
@@ -592,23 +592,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
     <col min="3" max="3" width="48.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -621,11 +622,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -636,554 +634,455 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>37</v>
       </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>39</v>
       </c>
-      <c r="D16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C18" t="s">
         <v>42</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
         <v>43</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>44</v>
       </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>46</v>
       </c>
-      <c r="D19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
         <v>47</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>48</v>
       </c>
-      <c r="D20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
         <v>51</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="D23" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>56</v>
       </c>
-      <c r="D24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
         <v>57</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>58</v>
       </c>
-      <c r="D25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>60</v>
       </c>
-      <c r="D26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
         <v>61</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>62</v>
       </c>
-      <c r="D27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
         <v>63</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>64</v>
       </c>
-      <c r="D28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="D29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
         <v>65</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
         <v>67</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
         <v>68</v>
       </c>
-      <c r="D30" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C32" t="s">
         <v>69</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D32" t="s">
         <v>70</v>
       </c>
-      <c r="D31" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
         <v>71</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>72</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
         <v>73</v>
       </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C34" t="s">
         <v>74</v>
       </c>
-      <c r="C33" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" t="s">
-        <v>77</v>
-      </c>
       <c r="D34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>